<commit_message>
menu() is not working properly
</commit_message>
<xml_diff>
--- a/shopingFile.xlsx
+++ b/shopingFile.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="630" yWindow="1710" windowWidth="15375" windowHeight="8325" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" state="visible" r:id="rId1"/>
@@ -392,7 +392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
@@ -434,14 +434,14 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>computer</t>
+          <t>Pen</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>10000</v>
+        <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>5</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3">
@@ -450,14 +450,14 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>pen</t>
+          <t>Computer</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>10000</v>
       </c>
       <c r="D3" t="n">
-        <v>1000</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -494,98 +494,194 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>mouse</t>
+          <t>Ipad</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ipad</t>
+          <t>mouse</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="D7" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>mouse</t>
+          <t>Keyboard</t>
         </is>
       </c>
       <c r="C8" t="n">
         <v>100</v>
       </c>
       <c r="D8" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Keyboard</t>
+          <t>Mouse</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D9" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Mouse</t>
+          <t>Smart watch</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>101</v>
+        <v>2000</v>
       </c>
       <c r="D10" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Smart watch</t>
+          <t>Hard disk</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2000</v>
+        <v>8000</v>
       </c>
       <c r="D11" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1014</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>SSD</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>2800</v>
+      </c>
+      <c r="D12" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1015</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>RAM</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>3500</v>
+      </c>
+      <c r="D13" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1016</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Monitor</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>15000</v>
+      </c>
+      <c r="D14" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Laptop table</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D15" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1018</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Cable</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>100</v>
+      </c>
+      <c r="D16" t="n">
+        <v>99950</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1019</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Wireless mouse</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D17" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -599,10 +695,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -730,6 +826,240 @@
         </is>
       </c>
       <c r="I3" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1011</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Mouse</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D4" t="n">
+        <v>101</v>
+      </c>
+      <c r="E4" t="n">
+        <v>808</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Barkatopu</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0180</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1012</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Smart watch</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E5" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>dip</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>fftgr</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>34435</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1012</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Smart watch</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E6" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Barkatopu</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>0180</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1013</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Barkatopu</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>0180</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1018</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Cable</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>50</v>
+      </c>
+      <c r="D8" t="n">
+        <v>100</v>
+      </c>
+      <c r="E8" t="n">
+        <v>5000</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Phone</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1019</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Wireless mouse</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Phone</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
         <is>
           <t>COD</t>
         </is>
@@ -746,10 +1076,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -762,13 +1092,204 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>User ID</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
           <t>Password</t>
         </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Phone</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mohammad Barkatullah </t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>barkatopu</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>01521</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Barkatopu</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>barkat1345</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0180</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mohammad </t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>barkat</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>foolan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Admin</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>xyz</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Barkat</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>boss</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>xzy</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>partho</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>partho123</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>fds</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>304585</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Alma</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>alma</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>xas</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>2432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
every funcitons are working perfectly. Now it is time to write the flow chart and report
</commit_message>
<xml_diff>
--- a/shopingFile.xlsx
+++ b/shopingFile.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="630" yWindow="1710" windowWidth="15375" windowHeight="8325" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,7 +17,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -47,8 +49,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,7 +395,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
@@ -478,210 +481,178 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1004</v>
+        <v>1007</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>pen drive</t>
+          <t>Ipad</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Ipad</t>
+          <t>mouse</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="D6" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>mouse</t>
+          <t>Keyboard</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D7" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Keyboard</t>
+          <t>Mouse</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Mouse</t>
+          <t>Hard disk</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>101</v>
+        <v>8000</v>
       </c>
       <c r="D9" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Smart watch</t>
+          <t>SSD</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2000</v>
+        <v>2800</v>
       </c>
       <c r="D10" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1013</v>
+        <v>1015</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Hard disk</t>
+          <t>RAM</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8000</v>
+        <v>4000</v>
       </c>
       <c r="D11" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SSD</t>
+          <t>Monitor</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>2800</v>
+        <v>15000</v>
       </c>
       <c r="D12" t="n">
-        <v>25</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1015</v>
+        <v>1018</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>RAM</t>
+          <t>Fiver cable</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>3500</v>
+        <v>100</v>
       </c>
       <c r="D13" t="n">
-        <v>25</v>
+        <v>998</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1016</v>
+        <v>1019</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Monitor</t>
+          <t>pen drive</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>15000</v>
+        <v>1000</v>
       </c>
       <c r="D14" t="n">
-        <v>5</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1017</v>
+        <v>1020</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Laptop table</t>
+          <t>Ups</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="D15" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>1018</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Cable</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>100</v>
-      </c>
-      <c r="D16" t="n">
-        <v>99950</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>1019</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Wireless mouse</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D17" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -695,10 +666,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -752,6 +723,11 @@
           <t>Payment Method</t>
         </is>
       </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -1060,6 +1036,438 @@
         </is>
       </c>
       <c r="I9" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1015</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>RAM</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>3500</v>
+      </c>
+      <c r="E10" t="n">
+        <v>7000</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Mohammad</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>fsdaf</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>431</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>bkash</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1015</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>RAM</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>3</v>
+      </c>
+      <c r="D11" t="n">
+        <v>3500</v>
+      </c>
+      <c r="E11" t="n">
+        <v>10500</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Mohammad Barkatullah</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>fsdf</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>44234</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1019</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Wireless mouse</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>3</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3000</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Mohammad</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>fdsf</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>4234</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nogod</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1020</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Bluetooth dangle</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" t="n">
+        <v>300</v>
+      </c>
+      <c r="E13" t="n">
+        <v>600</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Sadia Afroz</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>uttara</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>34324</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>bkash</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1018</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Fiver cable</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>10</v>
+      </c>
+      <c r="D14" t="n">
+        <v>105</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1050</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Israt Rimpi</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>fdsf</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>4324</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1018</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Fiver cable</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>10</v>
+      </c>
+      <c r="D15" t="n">
+        <v>105</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1050</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Partho</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>fsdf</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>41234</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1018</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Fiver cable</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>10</v>
+      </c>
+      <c r="D16" t="n">
+        <v>105</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1050</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Partho</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>fsdf</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>54324323425</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>nogod</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1011</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Mouse</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>3</v>
+      </c>
+      <c r="D17" t="n">
+        <v>101</v>
+      </c>
+      <c r="E17" t="n">
+        <v>303</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Dipanker</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>fsdf</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>4234</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>bkash</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="I18" s="1" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1007</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Ipad</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>2</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>sadia</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>uttara</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>32443</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>cod</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1020</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Ups</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" t="n">
+        <v>10000</v>
+      </c>
+      <c r="E20" t="n">
+        <v>20000</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Mohammad Barkatullah</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>fsdafasd</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>435</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1018</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Fiver cable</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>2</v>
+      </c>
+      <c r="D21" t="n">
+        <v>100</v>
+      </c>
+      <c r="E21" t="n">
+        <v>200</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Barkat</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>fdsf</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>5443124</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
         <is>
           <t>COD</t>
         </is>
@@ -1078,8 +1486,8 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1114,118 +1522,120 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mohammad Barkatullah </t>
+          <t xml:space="preserve">Mohammad </t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>barkatopu</t>
+          <t>barkat</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1234</t>
+          <t>123</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>abc</t>
+          <t>fsdf</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>01521</t>
+          <t>4324</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Barkatopu</t>
+          <t>Barkat</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>barkat1345</t>
+          <t>barkatopu</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1234</t>
+          <t>123</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>abc</t>
+          <t>fdsf</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0180</t>
+          <t>4324</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mohammad </t>
+          <t>Dip</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>barkat</t>
+          <t>dip</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>12345</t>
+          <t>123</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>foolan</t>
+          <t>vasfd</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>000000</t>
+          <t>4234</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Admin</t>
+          <t>partho</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Admin</t>
+          <t>partho</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1234</t>
+          <t>123</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>xyz</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
+          <t>fsdf</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>4324</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Barkat</t>
+          <t>Mohammad Barkatullah</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>boss</t>
+          <t>barkat1345</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1235,22 +1645,24 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>xzy</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
+          <t>xyz</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>01521206720</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>partho</t>
+          <t>Sadia afroz</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>partho123</t>
+          <t>sadia</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1260,22 +1672,24 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>fds</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>304585</v>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>543543</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Alma</t>
+          <t>Israt rimpi</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>alma</t>
+          <t>rimpi</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1285,11 +1699,13 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>xas</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>2432</v>
+          <t>uttara</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>341234</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
flow chart and code are done
</commit_message>
<xml_diff>
--- a/shopingFile.xlsx
+++ b/shopingFile.xlsx
@@ -395,7 +395,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="D3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -476,7 +476,7 @@
         <v>200</v>
       </c>
       <c r="D4" t="n">
-        <v>5000</v>
+        <v>4999</v>
       </c>
     </row>
     <row r="5">
@@ -561,66 +561,18 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>SSD</t>
+          <t>RAM</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2800</v>
+        <v>3000</v>
       </c>
       <c r="D10" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>1015</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>RAM</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>4000</v>
-      </c>
-      <c r="D11" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>1016</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Monitor</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>15000</v>
-      </c>
-      <c r="D12" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>1018</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Fiver cable</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>10</v>
-      </c>
-      <c r="D13" t="n">
-        <v>10000</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -634,7 +586,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
@@ -1558,6 +1510,201 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>1016</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Monitor</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" t="n">
+        <v>15000</v>
+      </c>
+      <c r="E25" t="n">
+        <v>30000</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Partho</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>fsdjhfg</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>54353</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>1015</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Ram</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>2</v>
+      </c>
+      <c r="D26" t="n">
+        <v>3000</v>
+      </c>
+      <c r="E26" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Partho12</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>fsdf</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>543523</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>nogod</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>1014</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>SSD</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>2</v>
+      </c>
+      <c r="D27" t="n">
+        <v>2800</v>
+      </c>
+      <c r="E27" t="n">
+        <v>5600</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Dipanker</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>fsdalfk</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>43532</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>1016</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>RAM</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" t="n">
+        <v>3000</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3000</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Safi ahmed</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>abv</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>54325</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>bkash</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>1002</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>mouse pad</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" t="n">
+        <v>200</v>
+      </c>
+      <c r="E29" t="n">
+        <v>200</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Safi</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>fsadf</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>32423</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1569,7 +1716,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
@@ -1820,6 +1967,87 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Saquib</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>saquib</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>fsdf</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>4324</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Safi</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>safi</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>fsdf</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>44234</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Saddam</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>saddam</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>fsdal;</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>453</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
in the code, discount, order id added. and menu() made more efficient. and word file updated with methods section
</commit_message>
<xml_diff>
--- a/shopingFile.xlsx
+++ b/shopingFile.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="975" yWindow="2055" windowWidth="15375" windowHeight="8325" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,8 +17,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/YYYY HH:MM:SS"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -49,9 +50,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,7 +398,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
@@ -444,7 +447,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3">
@@ -469,14 +472,14 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>mouse pad</t>
+          <t>Mouse Pad</t>
         </is>
       </c>
       <c r="C4" t="n">
         <v>200</v>
       </c>
       <c r="D4" t="n">
-        <v>4999</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="5">
@@ -492,7 +495,7 @@
         <v>1000</v>
       </c>
       <c r="D5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
@@ -501,14 +504,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>mouse</t>
+          <t>Bluetooth Mouse</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>300</v>
+        <v>1500</v>
       </c>
       <c r="D6" t="n">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
@@ -540,7 +543,7 @@
         <v>110</v>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
@@ -572,7 +575,71 @@
         <v>3000</v>
       </c>
       <c r="D10" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1018</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Fiver cable</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>10</v>
+      </c>
+      <c r="D11" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1020</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Membrane keyboard</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>300</v>
+      </c>
+      <c r="D12" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1022</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Gaming Headphone</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>4000</v>
+      </c>
+      <c r="D13" t="n">
         <v>19</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1023</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Smart Watch</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>11000</v>
+      </c>
+      <c r="D14" t="n">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -586,21 +653,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="16.42578125" bestFit="1" customWidth="1" min="9" max="9"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Product ID</t>
+          <t>Order ID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -651,1057 +715,355 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1011</v>
+        <v>1007</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mouse</t>
+          <t>Ipad</t>
         </is>
       </c>
       <c r="C2" t="n">
         <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>101</v>
+        <v>1000</v>
       </c>
       <c r="E2" t="n">
-        <v>202</v>
+        <v>2000</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>abc</t>
+          <t>Mohammad Barkatullah</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>dfda</t>
+          <t>Dhaka</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>01521202</t>
+          <t>4324</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
           <t>COD</t>
+        </is>
+      </c>
+      <c r="J2" s="2" t="inlineStr">
+        <is>
+          <t>03/09/2021 12-17-13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1009</v>
+        <v>1002</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Keyboard</t>
+          <t>mouse pad</t>
         </is>
       </c>
       <c r="C3" t="n">
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E3" t="n">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Mohammad Barkatullah</t>
+          <t xml:space="preserve">Dipanker </t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>abc</t>
+          <t>ctg</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>01453</t>
+          <t>3242</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>COD</t>
+          <t>bkash</t>
+        </is>
+      </c>
+      <c r="J3" s="3" t="inlineStr">
+        <is>
+          <t>03/09/2021 12-21-23</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1011</v>
+        <v>1007</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Mouse</t>
+          <t>Ipad</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>101</v>
+        <v>1000</v>
       </c>
       <c r="E4" t="n">
-        <v>808</v>
+        <v>1000</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Barkatopu</t>
+          <t>Saddam</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>abc</t>
+          <t>Bhola</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>0180</t>
+          <t>432432</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
           <t>COD</t>
+        </is>
+      </c>
+      <c r="J4" s="3" t="inlineStr">
+        <is>
+          <t>03/09/2021 12-31-02</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1012</v>
+        <v>1016</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Smart watch</t>
+          <t>RAM</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="E5" t="n">
         <v>6000</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>dip</t>
+          <t>Safi</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>fftgr</t>
+          <t>Dhaka</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>34435</t>
+          <t>345</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
           <t>COD</t>
+        </is>
+      </c>
+      <c r="J5" s="3" t="inlineStr">
+        <is>
+          <t>03/09/2021 12-33-59</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1012</v>
+        <v>1008</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Smart watch</t>
+          <t>Bluetooth Mouse</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="E6" t="n">
-        <v>6000</v>
+        <v>1474</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Barkatopu</t>
+          <t>Saddam</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>abc</t>
+          <t>Bhola</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>0180</t>
+          <t>54234</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
           <t>COD</t>
+        </is>
+      </c>
+      <c r="J6" s="3" t="inlineStr">
+        <is>
+          <t>03/09/2021 14-31-53</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1013</v>
+        <v>1022</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Gaming Headphone</t>
         </is>
       </c>
       <c r="C7" t="n">
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Barkatopu</t>
+          <t>Saddam</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>abc</t>
+          <t>Bhola</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>0180</t>
+          <t>5423</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>COD</t>
+          <t>nogod</t>
+        </is>
+      </c>
+      <c r="J7" s="3" t="inlineStr">
+        <is>
+          <t>03/09/2021 14-37-55</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1018</v>
+        <v>1002</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Cable</t>
+          <t>Mouse Pad</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E8" t="n">
-        <v>5000</v>
+        <v>182</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>Saddam</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Address</t>
+          <t>Bhola</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Phone</t>
+          <t>4324</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
+          <t>bkash</t>
+        </is>
+      </c>
+      <c r="J8" s="3" t="inlineStr">
+        <is>
+          <t>03/09/2021 14-38-32</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>03092021144022</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Mouse</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>110</v>
+      </c>
+      <c r="E9" t="n">
+        <v>34</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Barkat</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Dhaka</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>4324</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
           <t>COD</t>
         </is>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>1019</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Wireless mouse</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>2</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E9" t="n">
-        <v>2000</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Address</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Phone</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>COD</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>1015</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>RAM</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>2</v>
-      </c>
-      <c r="D10" t="n">
-        <v>3500</v>
-      </c>
-      <c r="E10" t="n">
-        <v>7000</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Mohammad</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>fsdaf</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>431</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>bkash</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>1015</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>RAM</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>3</v>
-      </c>
-      <c r="D11" t="n">
-        <v>3500</v>
-      </c>
-      <c r="E11" t="n">
-        <v>10500</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Mohammad Barkatullah</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>fsdf</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>44234</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>COD</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>1019</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Wireless mouse</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>3</v>
-      </c>
-      <c r="D12" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E12" t="n">
-        <v>3000</v>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Mohammad</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>fdsf</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>4234</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nogod</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>1020</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Bluetooth dangle</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>2</v>
-      </c>
-      <c r="D13" t="n">
-        <v>300</v>
-      </c>
-      <c r="E13" t="n">
-        <v>600</v>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Sadia Afroz</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>uttara</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>34324</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>bkash</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>1018</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Fiver cable</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>10</v>
-      </c>
-      <c r="D14" t="n">
-        <v>105</v>
-      </c>
-      <c r="E14" t="n">
-        <v>1050</v>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Israt Rimpi</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>fdsf</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>4324</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>COD</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>1018</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Fiver cable</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>10</v>
-      </c>
-      <c r="D15" t="n">
-        <v>105</v>
-      </c>
-      <c r="E15" t="n">
-        <v>1050</v>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Partho</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>fsdf</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>41234</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>COD</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>1018</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Fiver cable</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>10</v>
-      </c>
-      <c r="D16" t="n">
-        <v>105</v>
-      </c>
-      <c r="E16" t="n">
-        <v>1050</v>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Partho</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>fsdf</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>54324323425</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>nogod</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>1011</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Mouse</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>3</v>
-      </c>
-      <c r="D17" t="n">
-        <v>101</v>
-      </c>
-      <c r="E17" t="n">
-        <v>303</v>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Dipanker</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>fsdf</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>4234</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>bkash</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="I18" s="1" t="n"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>1007</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Ipad</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>2</v>
-      </c>
-      <c r="D19" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E19" t="n">
-        <v>2000</v>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>sadia</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>uttara</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>32443</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>cod</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>1020</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Ups</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>2</v>
-      </c>
-      <c r="D20" t="n">
-        <v>10000</v>
-      </c>
-      <c r="E20" t="n">
-        <v>20000</v>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Mohammad Barkatullah</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>fsdafasd</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>435</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>COD</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>1018</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Fiver cable</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>2</v>
-      </c>
-      <c r="D21" t="n">
-        <v>100</v>
-      </c>
-      <c r="E21" t="n">
-        <v>200</v>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Barkat</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>fdsf</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>5443124</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>COD</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>1000</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Pen</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>2</v>
-      </c>
-      <c r="D22" t="n">
-        <v>10</v>
-      </c>
-      <c r="E22" t="n">
-        <v>20</v>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Sadia afroz</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>fsdfsd</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>5435</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>nogod</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>1001</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Computer</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23" t="n">
-        <v>10000</v>
-      </c>
-      <c r="E23" t="n">
-        <v>10000</v>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Sadia</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>uttara</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>5435325</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>COD</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>1019</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Pen drive</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>2</v>
-      </c>
-      <c r="D24" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E24" t="n">
-        <v>2000</v>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Usrah saba</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>dflsaj</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>543534</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>bkash</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>1016</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Monitor</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>2</v>
-      </c>
-      <c r="D25" t="n">
-        <v>15000</v>
-      </c>
-      <c r="E25" t="n">
-        <v>30000</v>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Partho</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>fsdjhfg</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>54353</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>COD</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>1015</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Ram</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
-        <v>2</v>
-      </c>
-      <c r="D26" t="n">
-        <v>3000</v>
-      </c>
-      <c r="E26" t="n">
-        <v>6000</v>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Partho12</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>fsdf</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>543523</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>nogod</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>1014</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>SSD</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
-        <v>2</v>
-      </c>
-      <c r="D27" t="n">
-        <v>2800</v>
-      </c>
-      <c r="E27" t="n">
-        <v>5600</v>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>Dipanker</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>fsdalfk</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>43532</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>COD</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>1016</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>RAM</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
-        <v>1</v>
-      </c>
-      <c r="D28" t="n">
-        <v>3000</v>
-      </c>
-      <c r="E28" t="n">
-        <v>3000</v>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>Safi ahmed</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>abv</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>54325</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>bkash</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>1002</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>mouse pad</t>
-        </is>
-      </c>
-      <c r="C29" t="n">
-        <v>1</v>
-      </c>
-      <c r="D29" t="n">
-        <v>200</v>
-      </c>
-      <c r="E29" t="n">
-        <v>200</v>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>Safi</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>fsadf</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>32423</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>COD</t>
+      <c r="J9" s="3" t="inlineStr">
+        <is>
+          <t>03/09/2021 14-40-22</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Project is completed for now
</commit_message>
<xml_diff>
--- a/shopingFile.xlsx
+++ b/shopingFile.xlsx
@@ -1078,7 +1078,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
@@ -1410,6 +1410,33 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Mustafa kamal</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>mustafa</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>fdsf</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>45325</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
deleteOrder() has been added
</commit_message>
<xml_diff>
--- a/shopingFile.xlsx
+++ b/shopingFile.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="975" yWindow="2055" windowWidth="15375" windowHeight="8325" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="975" yWindow="2055" windowWidth="15375" windowHeight="8325" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="soldProduct" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="userAccount" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="userAccount" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="soldProduct" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -17,9 +17,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/YYYY HH:MM:SS"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/YYYY HH:MM:SS"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -50,11 +49,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,7 +444,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3">
@@ -511,7 +508,7 @@
         <v>1500</v>
       </c>
       <c r="D6" t="n">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7">
@@ -527,7 +524,7 @@
         <v>100</v>
       </c>
       <c r="D7" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
@@ -543,7 +540,7 @@
         <v>110</v>
       </c>
       <c r="D8" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9">
@@ -575,7 +572,7 @@
         <v>3000</v>
       </c>
       <c r="D10" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11">
@@ -607,7 +604,7 @@
         <v>300</v>
       </c>
       <c r="D12" t="n">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13">
@@ -648,431 +645,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Order ID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Product Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Unit price</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>address</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>phone</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Payment Method</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1007</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Ipad</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Mohammad Barkatullah</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Dhaka</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>4324</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>COD</t>
-        </is>
-      </c>
-      <c r="J2" s="2" t="inlineStr">
-        <is>
-          <t>03/09/2021 12-17-13</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1002</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>mouse pad</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="n">
-        <v>200</v>
-      </c>
-      <c r="E3" t="n">
-        <v>400</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Dipanker </t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>ctg</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>3242</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>bkash</t>
-        </is>
-      </c>
-      <c r="J3" s="3" t="inlineStr">
-        <is>
-          <t>03/09/2021 12-21-23</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1007</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Ipad</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Saddam</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Bhola</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>432432</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>COD</t>
-        </is>
-      </c>
-      <c r="J4" s="3" t="inlineStr">
-        <is>
-          <t>03/09/2021 12-31-02</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1016</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>RAM</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" t="n">
-        <v>3000</v>
-      </c>
-      <c r="E5" t="n">
-        <v>6000</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Safi</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Dhaka</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>345</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>COD</t>
-        </is>
-      </c>
-      <c r="J5" s="3" t="inlineStr">
-        <is>
-          <t>03/09/2021 12-33-59</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>1008</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Bluetooth Mouse</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1500</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1474</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Saddam</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Bhola</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>54234</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>COD</t>
-        </is>
-      </c>
-      <c r="J6" s="3" t="inlineStr">
-        <is>
-          <t>03/09/2021 14-31-53</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>1022</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Gaming Headphone</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>4000</v>
-      </c>
-      <c r="E7" t="n">
-        <v>4000</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Saddam</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Bhola</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>5423</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nogod</t>
-        </is>
-      </c>
-      <c r="J7" s="3" t="inlineStr">
-        <is>
-          <t>03/09/2021 14-37-55</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>1002</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Mouse Pad</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" t="n">
-        <v>200</v>
-      </c>
-      <c r="E8" t="n">
-        <v>182</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Saddam</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Bhola</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>4324</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>bkash</t>
-        </is>
-      </c>
-      <c r="J8" s="3" t="inlineStr">
-        <is>
-          <t>03/09/2021 14-38-32</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>03092021144022</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Mouse</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" t="n">
-        <v>110</v>
-      </c>
-      <c r="E9" t="n">
-        <v>34</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Barkat</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Dhaka</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>4324</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>COD</t>
-        </is>
-      </c>
-      <c r="J9" s="3" t="inlineStr">
-        <is>
-          <t>03/09/2021 14-40-22</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1440,4 +1012,288 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Order ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Product Name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Unit price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>User Id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>address</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>phone</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Payment Method</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>05092021144441</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Computer</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>100000</v>
+      </c>
+      <c r="E2" t="n">
+        <v>99971</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>saddam</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Saddam</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>bhola</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>44324</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>bkash</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>05/09/2021 14-44-41</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>05092021144536</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Bluetooth Mouse</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1500</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2943</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>partho</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Partho</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>fsdaf</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>4324</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nogod</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>05/09/2021 14-45-36</t>
+        </is>
+      </c>
+      <c r="L3" s="1" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>05092021144616</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>RAM</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3000</v>
+      </c>
+      <c r="E4" t="n">
+        <v>9000</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>dip</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Dipanker</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>ctg</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>07987</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>05/09/2021 14-46-16</t>
+        </is>
+      </c>
+      <c r="L4" s="1" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>05092021153317</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Mouse</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>110</v>
+      </c>
+      <c r="E5" t="n">
+        <v>322</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>sadia</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Sadia</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>uttara</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>454</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nogod</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>05/09/2021 15-33-17</t>
+        </is>
+      </c>
+      <c r="L5" s="1" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>